<commit_message>
adding 2018 midterm data, new output
</commit_message>
<xml_diff>
--- a/Projects/Voter Turnout Analysis/data/voter turnout by age and ideology.xlsx
+++ b/Projects/Voter Turnout Analysis/data/voter turnout by age and ideology.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Public_Policy\Projects\Voter Turnout Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD06A410-ABE8-4A43-9EA2-0A5606A85D2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61951B95-0A70-4A4C-8A0E-9F8AE13CCA85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clean table" sheetId="2" r:id="rId1"/>
     <sheet name="age stats" sheetId="1" r:id="rId2"/>
     <sheet name="exit poll data" sheetId="3" r:id="rId3"/>
-    <sheet name="partisan lean data" sheetId="4" r:id="rId4"/>
-    <sheet name="age by indv years" sheetId="5" r:id="rId5"/>
-    <sheet name="lean_data_clean" sheetId="6" r:id="rId6"/>
+    <sheet name="2018 nov midterm reg turnout" sheetId="8" r:id="rId4"/>
+    <sheet name="partisan lean data" sheetId="4" r:id="rId5"/>
+    <sheet name="age by indv years" sheetId="5" r:id="rId6"/>
+    <sheet name="lean_data_clean" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="238">
   <si>
     <t>United States</t>
   </si>
@@ -647,19 +648,148 @@
   </si>
   <si>
     <t>Share of Voting Age Pop</t>
+  </si>
+  <si>
+    <t>United States citizen</t>
+  </si>
+  <si>
+    <t>Total citizen population</t>
+  </si>
+  <si>
+    <t>Reported registered</t>
+  </si>
+  <si>
+    <t>Reported not registered</t>
+  </si>
+  <si>
+    <r>
+      <t>No response to registration</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+  </si>
+  <si>
+    <t>Reported voted</t>
+  </si>
+  <si>
+    <t>Reported not voted</t>
+  </si>
+  <si>
+    <r>
+      <t>No response to voting</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>25 to 34 years</t>
+  </si>
+  <si>
+    <t>35 to 44 years</t>
+  </si>
+  <si>
+    <t>45 to 54 years</t>
+  </si>
+  <si>
+    <t>55 to 64 years</t>
+  </si>
+  <si>
+    <t>65 to 74 years</t>
+  </si>
+  <si>
+    <t>80-84</t>
+  </si>
+  <si>
+    <t>85 and over</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>total pop</t>
+  </si>
+  <si>
+    <t>citizen pop</t>
+  </si>
+  <si>
+    <t>citizen registered</t>
+  </si>
+  <si>
+    <t>pct citizen registered</t>
+  </si>
+  <si>
+    <t>citizen not registered</t>
+  </si>
+  <si>
+    <t>pct citizen not registered</t>
+  </si>
+  <si>
+    <t>citizen no reg response</t>
+  </si>
+  <si>
+    <t>citizen pct no reg response</t>
+  </si>
+  <si>
+    <t>citizen voted</t>
+  </si>
+  <si>
+    <t>citizen pct voted</t>
+  </si>
+  <si>
+    <t>citizen no vote response</t>
+  </si>
+  <si>
+    <t>citizen no vote</t>
+  </si>
+  <si>
+    <t>citizen pct no vote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citizen pct no vote response </t>
+  </si>
+  <si>
+    <t>pop pct registered</t>
+  </si>
+  <si>
+    <t>pop pct voted</t>
+  </si>
+  <si>
+    <t>80+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,6 +928,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -981,7 +1125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1096,6 +1240,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1144,7 +1303,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1163,6 +1322,29 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1665,7 +1847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDD4C4E-1AD3-4CD0-AFFF-3F372C3B1089}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1997,9 +2179,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV45"/>
+  <dimension ref="A1:AV53"/>
   <sheetViews>
-    <sheetView topLeftCell="H19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView topLeftCell="H19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y52" sqref="Y52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4324,6 +4508,41 @@
         <v>11</v>
       </c>
     </row>
+    <row r="47" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U47" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U48" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="21:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U49" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="21:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U50" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="21:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U51" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="21:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U52" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="21:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U53" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4357,6 +4576,3660 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5335A444-C933-4603-8804-D9B90131DA75}">
+  <dimension ref="A1:Q69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B5:B69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="21"/>
+    <col min="2" max="3" width="10.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9" style="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="15"/>
+    </row>
+    <row r="2" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
+        <v>18</v>
+      </c>
+      <c r="B5" s="19">
+        <v>4045</v>
+      </c>
+      <c r="C5" s="19">
+        <v>3823</v>
+      </c>
+      <c r="D5" s="19">
+        <v>1279</v>
+      </c>
+      <c r="E5" s="20">
+        <v>33.5</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1310</v>
+      </c>
+      <c r="G5" s="20">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="H5" s="19">
+        <v>1234</v>
+      </c>
+      <c r="I5" s="20">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="J5" s="19">
+        <v>919</v>
+      </c>
+      <c r="K5" s="20">
+        <v>24</v>
+      </c>
+      <c r="L5" s="19">
+        <v>1771</v>
+      </c>
+      <c r="M5" s="20">
+        <v>46.3</v>
+      </c>
+      <c r="N5" s="19">
+        <v>1132</v>
+      </c>
+      <c r="O5" s="20">
+        <v>29.6</v>
+      </c>
+      <c r="P5" s="20">
+        <v>31.6</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>19</v>
+      </c>
+      <c r="B6" s="19">
+        <v>3759</v>
+      </c>
+      <c r="C6" s="19">
+        <v>3561</v>
+      </c>
+      <c r="D6" s="19">
+        <v>1561</v>
+      </c>
+      <c r="E6" s="20">
+        <v>43.8</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1126</v>
+      </c>
+      <c r="G6" s="20">
+        <v>31.6</v>
+      </c>
+      <c r="H6" s="19">
+        <v>874</v>
+      </c>
+      <c r="I6" s="20">
+        <v>24.5</v>
+      </c>
+      <c r="J6" s="19">
+        <v>1068</v>
+      </c>
+      <c r="K6" s="20">
+        <v>30</v>
+      </c>
+      <c r="L6" s="19">
+        <v>1695</v>
+      </c>
+      <c r="M6" s="20">
+        <v>47.6</v>
+      </c>
+      <c r="N6" s="19">
+        <v>798</v>
+      </c>
+      <c r="O6" s="20">
+        <v>22.4</v>
+      </c>
+      <c r="P6" s="20">
+        <v>41.5</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
+        <v>20</v>
+      </c>
+      <c r="B7" s="19">
+        <v>4218</v>
+      </c>
+      <c r="C7" s="19">
+        <v>3910</v>
+      </c>
+      <c r="D7" s="19">
+        <v>2064</v>
+      </c>
+      <c r="E7" s="20">
+        <v>52.8</v>
+      </c>
+      <c r="F7" s="19">
+        <v>1011</v>
+      </c>
+      <c r="G7" s="20">
+        <v>25.9</v>
+      </c>
+      <c r="H7" s="19">
+        <v>835</v>
+      </c>
+      <c r="I7" s="20">
+        <v>21.4</v>
+      </c>
+      <c r="J7" s="19">
+        <v>1283</v>
+      </c>
+      <c r="K7" s="20">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="L7" s="19">
+        <v>1812</v>
+      </c>
+      <c r="M7" s="20">
+        <v>46.3</v>
+      </c>
+      <c r="N7" s="19">
+        <v>815</v>
+      </c>
+      <c r="O7" s="20">
+        <v>20.8</v>
+      </c>
+      <c r="P7" s="20">
+        <v>48.9</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
+        <v>21</v>
+      </c>
+      <c r="B8" s="19">
+        <v>4125</v>
+      </c>
+      <c r="C8" s="19">
+        <v>3849</v>
+      </c>
+      <c r="D8" s="19">
+        <v>1983</v>
+      </c>
+      <c r="E8" s="20">
+        <v>51.5</v>
+      </c>
+      <c r="F8" s="19">
+        <v>875</v>
+      </c>
+      <c r="G8" s="20">
+        <v>22.7</v>
+      </c>
+      <c r="H8" s="19">
+        <v>991</v>
+      </c>
+      <c r="I8" s="20">
+        <v>25.7</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1262</v>
+      </c>
+      <c r="K8" s="20">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="L8" s="19">
+        <v>1591</v>
+      </c>
+      <c r="M8" s="20">
+        <v>41.3</v>
+      </c>
+      <c r="N8" s="19">
+        <v>996</v>
+      </c>
+      <c r="O8" s="20">
+        <v>25.9</v>
+      </c>
+      <c r="P8" s="20">
+        <v>48.1</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>22</v>
+      </c>
+      <c r="B9" s="19">
+        <v>4152</v>
+      </c>
+      <c r="C9" s="19">
+        <v>3819</v>
+      </c>
+      <c r="D9" s="19">
+        <v>2006</v>
+      </c>
+      <c r="E9" s="20">
+        <v>52.5</v>
+      </c>
+      <c r="F9" s="19">
+        <v>855</v>
+      </c>
+      <c r="G9" s="20">
+        <v>22.4</v>
+      </c>
+      <c r="H9" s="19">
+        <v>958</v>
+      </c>
+      <c r="I9" s="20">
+        <v>25.1</v>
+      </c>
+      <c r="J9" s="19">
+        <v>1359</v>
+      </c>
+      <c r="K9" s="20">
+        <v>35.6</v>
+      </c>
+      <c r="L9" s="19">
+        <v>1598</v>
+      </c>
+      <c r="M9" s="20">
+        <v>41.8</v>
+      </c>
+      <c r="N9" s="19">
+        <v>862</v>
+      </c>
+      <c r="O9" s="20">
+        <v>22.6</v>
+      </c>
+      <c r="P9" s="20">
+        <v>48.3</v>
+      </c>
+      <c r="Q9" s="20">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
+        <v>23</v>
+      </c>
+      <c r="B10" s="19">
+        <v>4312</v>
+      </c>
+      <c r="C10" s="19">
+        <v>3957</v>
+      </c>
+      <c r="D10" s="19">
+        <v>2191</v>
+      </c>
+      <c r="E10" s="20">
+        <v>55.4</v>
+      </c>
+      <c r="F10" s="19">
+        <v>833</v>
+      </c>
+      <c r="G10" s="20">
+        <v>21.1</v>
+      </c>
+      <c r="H10" s="19">
+        <v>933</v>
+      </c>
+      <c r="I10" s="20">
+        <v>23.6</v>
+      </c>
+      <c r="J10" s="19">
+        <v>1421</v>
+      </c>
+      <c r="K10" s="20">
+        <v>35.9</v>
+      </c>
+      <c r="L10" s="19">
+        <v>1619</v>
+      </c>
+      <c r="M10" s="20">
+        <v>40.9</v>
+      </c>
+      <c r="N10" s="19">
+        <v>916</v>
+      </c>
+      <c r="O10" s="20">
+        <v>23.2</v>
+      </c>
+      <c r="P10" s="20">
+        <v>50.8</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
+        <v>24</v>
+      </c>
+      <c r="B11" s="19">
+        <v>4383</v>
+      </c>
+      <c r="C11" s="19">
+        <v>4032</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2157</v>
+      </c>
+      <c r="E11" s="20">
+        <v>53.5</v>
+      </c>
+      <c r="F11" s="19">
+        <v>936</v>
+      </c>
+      <c r="G11" s="20">
+        <v>23.2</v>
+      </c>
+      <c r="H11" s="19">
+        <v>939</v>
+      </c>
+      <c r="I11" s="20">
+        <v>23.3</v>
+      </c>
+      <c r="J11" s="19">
+        <v>1413</v>
+      </c>
+      <c r="K11" s="20">
+        <v>35.1</v>
+      </c>
+      <c r="L11" s="19">
+        <v>1716</v>
+      </c>
+      <c r="M11" s="20">
+        <v>42.6</v>
+      </c>
+      <c r="N11" s="19">
+        <v>902</v>
+      </c>
+      <c r="O11" s="20">
+        <v>22.4</v>
+      </c>
+      <c r="P11" s="20">
+        <v>49.2</v>
+      </c>
+      <c r="Q11" s="20">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
+        <v>25</v>
+      </c>
+      <c r="B12" s="19">
+        <v>4434</v>
+      </c>
+      <c r="C12" s="19">
+        <v>3970</v>
+      </c>
+      <c r="D12" s="19">
+        <v>2171</v>
+      </c>
+      <c r="E12" s="20">
+        <v>54.7</v>
+      </c>
+      <c r="F12" s="19">
+        <v>788</v>
+      </c>
+      <c r="G12" s="20">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H12" s="19">
+        <v>1010</v>
+      </c>
+      <c r="I12" s="20">
+        <v>25.4</v>
+      </c>
+      <c r="J12" s="19">
+        <v>1469</v>
+      </c>
+      <c r="K12" s="20">
+        <v>37</v>
+      </c>
+      <c r="L12" s="19">
+        <v>1570</v>
+      </c>
+      <c r="M12" s="20">
+        <v>39.5</v>
+      </c>
+      <c r="N12" s="19">
+        <v>931</v>
+      </c>
+      <c r="O12" s="20">
+        <v>23.5</v>
+      </c>
+      <c r="P12" s="20">
+        <v>49</v>
+      </c>
+      <c r="Q12" s="20">
+        <v>33.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
+        <v>26</v>
+      </c>
+      <c r="B13" s="19">
+        <v>4495</v>
+      </c>
+      <c r="C13" s="19">
+        <v>4056</v>
+      </c>
+      <c r="D13" s="19">
+        <v>2291</v>
+      </c>
+      <c r="E13" s="20">
+        <v>56.5</v>
+      </c>
+      <c r="F13" s="19">
+        <v>900</v>
+      </c>
+      <c r="G13" s="20">
+        <v>22.2</v>
+      </c>
+      <c r="H13" s="19">
+        <v>865</v>
+      </c>
+      <c r="I13" s="20">
+        <v>21.3</v>
+      </c>
+      <c r="J13" s="19">
+        <v>1521</v>
+      </c>
+      <c r="K13" s="20">
+        <v>37.5</v>
+      </c>
+      <c r="L13" s="19">
+        <v>1653</v>
+      </c>
+      <c r="M13" s="20">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="N13" s="19">
+        <v>882</v>
+      </c>
+      <c r="O13" s="20">
+        <v>21.7</v>
+      </c>
+      <c r="P13" s="20">
+        <v>51</v>
+      </c>
+      <c r="Q13" s="20">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
+        <v>27</v>
+      </c>
+      <c r="B14" s="19">
+        <v>4489</v>
+      </c>
+      <c r="C14" s="19">
+        <v>3991</v>
+      </c>
+      <c r="D14" s="19">
+        <v>2368</v>
+      </c>
+      <c r="E14" s="20">
+        <v>59.3</v>
+      </c>
+      <c r="F14" s="19">
+        <v>812</v>
+      </c>
+      <c r="G14" s="20">
+        <v>20.3</v>
+      </c>
+      <c r="H14" s="19">
+        <v>811</v>
+      </c>
+      <c r="I14" s="20">
+        <v>20.3</v>
+      </c>
+      <c r="J14" s="19">
+        <v>1630</v>
+      </c>
+      <c r="K14" s="20">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="L14" s="19">
+        <v>1579</v>
+      </c>
+      <c r="M14" s="20">
+        <v>39.6</v>
+      </c>
+      <c r="N14" s="19">
+        <v>782</v>
+      </c>
+      <c r="O14" s="20">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="P14" s="20">
+        <v>52.8</v>
+      </c>
+      <c r="Q14" s="20">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>28</v>
+      </c>
+      <c r="B15" s="19">
+        <v>4887</v>
+      </c>
+      <c r="C15" s="19">
+        <v>4369</v>
+      </c>
+      <c r="D15" s="19">
+        <v>2569</v>
+      </c>
+      <c r="E15" s="20">
+        <v>58.8</v>
+      </c>
+      <c r="F15" s="19">
+        <v>841</v>
+      </c>
+      <c r="G15" s="20">
+        <v>19.2</v>
+      </c>
+      <c r="H15" s="19">
+        <v>959</v>
+      </c>
+      <c r="I15" s="20">
+        <v>22</v>
+      </c>
+      <c r="J15" s="19">
+        <v>1797</v>
+      </c>
+      <c r="K15" s="20">
+        <v>41.1</v>
+      </c>
+      <c r="L15" s="19">
+        <v>1627</v>
+      </c>
+      <c r="M15" s="20">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="N15" s="19">
+        <v>946</v>
+      </c>
+      <c r="O15" s="20">
+        <v>21.6</v>
+      </c>
+      <c r="P15" s="20">
+        <v>52.6</v>
+      </c>
+      <c r="Q15" s="20">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
+        <v>29</v>
+      </c>
+      <c r="B16" s="19">
+        <v>4693</v>
+      </c>
+      <c r="C16" s="19">
+        <v>4132</v>
+      </c>
+      <c r="D16" s="19">
+        <v>2488</v>
+      </c>
+      <c r="E16" s="20">
+        <v>60.2</v>
+      </c>
+      <c r="F16" s="19">
+        <v>805</v>
+      </c>
+      <c r="G16" s="20">
+        <v>19.5</v>
+      </c>
+      <c r="H16" s="19">
+        <v>838</v>
+      </c>
+      <c r="I16" s="20">
+        <v>20.3</v>
+      </c>
+      <c r="J16" s="19">
+        <v>1742</v>
+      </c>
+      <c r="K16" s="20">
+        <v>42.2</v>
+      </c>
+      <c r="L16" s="19">
+        <v>1610</v>
+      </c>
+      <c r="M16" s="20">
+        <v>39</v>
+      </c>
+      <c r="N16" s="19">
+        <v>780</v>
+      </c>
+      <c r="O16" s="20">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="P16" s="20">
+        <v>53</v>
+      </c>
+      <c r="Q16" s="20">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>30</v>
+      </c>
+      <c r="B17" s="19">
+        <v>4480</v>
+      </c>
+      <c r="C17" s="19">
+        <v>3905</v>
+      </c>
+      <c r="D17" s="19">
+        <v>2279</v>
+      </c>
+      <c r="E17" s="20">
+        <v>58.4</v>
+      </c>
+      <c r="F17" s="19">
+        <v>795</v>
+      </c>
+      <c r="G17" s="20">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H17" s="19">
+        <v>830</v>
+      </c>
+      <c r="I17" s="20">
+        <v>21.3</v>
+      </c>
+      <c r="J17" s="19">
+        <v>1631</v>
+      </c>
+      <c r="K17" s="20">
+        <v>41.8</v>
+      </c>
+      <c r="L17" s="19">
+        <v>1455</v>
+      </c>
+      <c r="M17" s="20">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="N17" s="19">
+        <v>818</v>
+      </c>
+      <c r="O17" s="20">
+        <v>21</v>
+      </c>
+      <c r="P17" s="20">
+        <v>50.9</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
+        <v>31</v>
+      </c>
+      <c r="B18" s="19">
+        <v>4011</v>
+      </c>
+      <c r="C18" s="19">
+        <v>3487</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1982</v>
+      </c>
+      <c r="E18" s="20">
+        <v>56.8</v>
+      </c>
+      <c r="F18" s="19">
+        <v>808</v>
+      </c>
+      <c r="G18" s="20">
+        <v>23.2</v>
+      </c>
+      <c r="H18" s="19">
+        <v>697</v>
+      </c>
+      <c r="I18" s="20">
+        <v>20</v>
+      </c>
+      <c r="J18" s="19">
+        <v>1483</v>
+      </c>
+      <c r="K18" s="20">
+        <v>42.5</v>
+      </c>
+      <c r="L18" s="19">
+        <v>1385</v>
+      </c>
+      <c r="M18" s="20">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="N18" s="19">
+        <v>619</v>
+      </c>
+      <c r="O18" s="20">
+        <v>17.8</v>
+      </c>
+      <c r="P18" s="20">
+        <v>49.4</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>32</v>
+      </c>
+      <c r="B19" s="19">
+        <v>4536</v>
+      </c>
+      <c r="C19" s="19">
+        <v>3870</v>
+      </c>
+      <c r="D19" s="19">
+        <v>2445</v>
+      </c>
+      <c r="E19" s="20">
+        <v>63.2</v>
+      </c>
+      <c r="F19" s="19">
+        <v>658</v>
+      </c>
+      <c r="G19" s="20">
+        <v>17</v>
+      </c>
+      <c r="H19" s="19">
+        <v>768</v>
+      </c>
+      <c r="I19" s="20">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="J19" s="19">
+        <v>1768</v>
+      </c>
+      <c r="K19" s="20">
+        <v>45.7</v>
+      </c>
+      <c r="L19" s="19">
+        <v>1349</v>
+      </c>
+      <c r="M19" s="20">
+        <v>34.9</v>
+      </c>
+      <c r="N19" s="19">
+        <v>753</v>
+      </c>
+      <c r="O19" s="20">
+        <v>19.5</v>
+      </c>
+      <c r="P19" s="20">
+        <v>53.9</v>
+      </c>
+      <c r="Q19" s="20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>33</v>
+      </c>
+      <c r="B20" s="19">
+        <v>4530</v>
+      </c>
+      <c r="C20" s="19">
+        <v>3875</v>
+      </c>
+      <c r="D20" s="19">
+        <v>2439</v>
+      </c>
+      <c r="E20" s="20">
+        <v>63</v>
+      </c>
+      <c r="F20" s="19">
+        <v>750</v>
+      </c>
+      <c r="G20" s="20">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="H20" s="19">
+        <v>685</v>
+      </c>
+      <c r="I20" s="20">
+        <v>17.7</v>
+      </c>
+      <c r="J20" s="19">
+        <v>1805</v>
+      </c>
+      <c r="K20" s="20">
+        <v>46.6</v>
+      </c>
+      <c r="L20" s="19">
+        <v>1420</v>
+      </c>
+      <c r="M20" s="20">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="N20" s="19">
+        <v>649</v>
+      </c>
+      <c r="O20" s="20">
+        <v>16.8</v>
+      </c>
+      <c r="P20" s="20">
+        <v>53.8</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="18">
+        <v>34</v>
+      </c>
+      <c r="B21" s="19">
+        <v>4214</v>
+      </c>
+      <c r="C21" s="19">
+        <v>3625</v>
+      </c>
+      <c r="D21" s="19">
+        <v>2309</v>
+      </c>
+      <c r="E21" s="20">
+        <v>63.7</v>
+      </c>
+      <c r="F21" s="19">
+        <v>651</v>
+      </c>
+      <c r="G21" s="20">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="H21" s="19">
+        <v>666</v>
+      </c>
+      <c r="I21" s="20">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="J21" s="19">
+        <v>1700</v>
+      </c>
+      <c r="K21" s="20">
+        <v>46.9</v>
+      </c>
+      <c r="L21" s="19">
+        <v>1281</v>
+      </c>
+      <c r="M21" s="20">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="N21" s="19">
+        <v>644</v>
+      </c>
+      <c r="O21" s="20">
+        <v>17.8</v>
+      </c>
+      <c r="P21" s="20">
+        <v>54.8</v>
+      </c>
+      <c r="Q21" s="20">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
+        <v>35</v>
+      </c>
+      <c r="B22" s="19">
+        <v>4103</v>
+      </c>
+      <c r="C22" s="19">
+        <v>3518</v>
+      </c>
+      <c r="D22" s="19">
+        <v>2292</v>
+      </c>
+      <c r="E22" s="20">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="F22" s="19">
+        <v>615</v>
+      </c>
+      <c r="G22" s="20">
+        <v>17.5</v>
+      </c>
+      <c r="H22" s="19">
+        <v>612</v>
+      </c>
+      <c r="I22" s="20">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J22" s="19">
+        <v>1701</v>
+      </c>
+      <c r="K22" s="20">
+        <v>48.3</v>
+      </c>
+      <c r="L22" s="19">
+        <v>1215</v>
+      </c>
+      <c r="M22" s="20">
+        <v>34.5</v>
+      </c>
+      <c r="N22" s="19">
+        <v>602</v>
+      </c>
+      <c r="O22" s="20">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="P22" s="20">
+        <v>55.9</v>
+      </c>
+      <c r="Q22" s="20">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="18">
+        <v>36</v>
+      </c>
+      <c r="B23" s="19">
+        <v>4375</v>
+      </c>
+      <c r="C23" s="19">
+        <v>3749</v>
+      </c>
+      <c r="D23" s="19">
+        <v>2367</v>
+      </c>
+      <c r="E23" s="20">
+        <v>63.1</v>
+      </c>
+      <c r="F23" s="19">
+        <v>636</v>
+      </c>
+      <c r="G23" s="20">
+        <v>17</v>
+      </c>
+      <c r="H23" s="19">
+        <v>747</v>
+      </c>
+      <c r="I23" s="20">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="J23" s="19">
+        <v>1746</v>
+      </c>
+      <c r="K23" s="20">
+        <v>46.6</v>
+      </c>
+      <c r="L23" s="19">
+        <v>1299</v>
+      </c>
+      <c r="M23" s="20">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="N23" s="19">
+        <v>704</v>
+      </c>
+      <c r="O23" s="20">
+        <v>18.8</v>
+      </c>
+      <c r="P23" s="20">
+        <v>54.1</v>
+      </c>
+      <c r="Q23" s="20">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="18">
+        <v>37</v>
+      </c>
+      <c r="B24" s="19">
+        <v>4281</v>
+      </c>
+      <c r="C24" s="19">
+        <v>3754</v>
+      </c>
+      <c r="D24" s="19">
+        <v>2500</v>
+      </c>
+      <c r="E24" s="20">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="F24" s="19">
+        <v>581</v>
+      </c>
+      <c r="G24" s="20">
+        <v>15.5</v>
+      </c>
+      <c r="H24" s="19">
+        <v>673</v>
+      </c>
+      <c r="I24" s="20">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="J24" s="19">
+        <v>1891</v>
+      </c>
+      <c r="K24" s="20">
+        <v>50.4</v>
+      </c>
+      <c r="L24" s="19">
+        <v>1231</v>
+      </c>
+      <c r="M24" s="20">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="N24" s="19">
+        <v>632</v>
+      </c>
+      <c r="O24" s="20">
+        <v>16.8</v>
+      </c>
+      <c r="P24" s="20">
+        <v>58.4</v>
+      </c>
+      <c r="Q24" s="20">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="18">
+        <v>38</v>
+      </c>
+      <c r="B25" s="19">
+        <v>4348</v>
+      </c>
+      <c r="C25" s="19">
+        <v>3799</v>
+      </c>
+      <c r="D25" s="19">
+        <v>2507</v>
+      </c>
+      <c r="E25" s="20">
+        <v>66</v>
+      </c>
+      <c r="F25" s="19">
+        <v>543</v>
+      </c>
+      <c r="G25" s="20">
+        <v>14.3</v>
+      </c>
+      <c r="H25" s="19">
+        <v>749</v>
+      </c>
+      <c r="I25" s="20">
+        <v>19.7</v>
+      </c>
+      <c r="J25" s="19">
+        <v>1896</v>
+      </c>
+      <c r="K25" s="20">
+        <v>49.9</v>
+      </c>
+      <c r="L25" s="19">
+        <v>1195</v>
+      </c>
+      <c r="M25" s="20">
+        <v>31.5</v>
+      </c>
+      <c r="N25" s="19">
+        <v>708</v>
+      </c>
+      <c r="O25" s="20">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="P25" s="20">
+        <v>57.7</v>
+      </c>
+      <c r="Q25" s="20">
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="18">
+        <v>39</v>
+      </c>
+      <c r="B26" s="19">
+        <v>4163</v>
+      </c>
+      <c r="C26" s="19">
+        <v>3663</v>
+      </c>
+      <c r="D26" s="19">
+        <v>2399</v>
+      </c>
+      <c r="E26" s="20">
+        <v>65.5</v>
+      </c>
+      <c r="F26" s="19">
+        <v>599</v>
+      </c>
+      <c r="G26" s="20">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="H26" s="19">
+        <v>665</v>
+      </c>
+      <c r="I26" s="20">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="J26" s="19">
+        <v>1872</v>
+      </c>
+      <c r="K26" s="20">
+        <v>51.1</v>
+      </c>
+      <c r="L26" s="19">
+        <v>1163</v>
+      </c>
+      <c r="M26" s="20">
+        <v>31.7</v>
+      </c>
+      <c r="N26" s="19">
+        <v>628</v>
+      </c>
+      <c r="O26" s="20">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="P26" s="20">
+        <v>57.6</v>
+      </c>
+      <c r="Q26" s="20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
+        <v>40</v>
+      </c>
+      <c r="B27" s="19">
+        <v>3935</v>
+      </c>
+      <c r="C27" s="19">
+        <v>3356</v>
+      </c>
+      <c r="D27" s="19">
+        <v>2170</v>
+      </c>
+      <c r="E27" s="20">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F27" s="19">
+        <v>472</v>
+      </c>
+      <c r="G27" s="20">
+        <v>14.1</v>
+      </c>
+      <c r="H27" s="19">
+        <v>715</v>
+      </c>
+      <c r="I27" s="20">
+        <v>21.3</v>
+      </c>
+      <c r="J27" s="19">
+        <v>1695</v>
+      </c>
+      <c r="K27" s="20">
+        <v>50.5</v>
+      </c>
+      <c r="L27" s="19">
+        <v>983</v>
+      </c>
+      <c r="M27" s="20">
+        <v>29.3</v>
+      </c>
+      <c r="N27" s="19">
+        <v>678</v>
+      </c>
+      <c r="O27" s="20">
+        <v>20.2</v>
+      </c>
+      <c r="P27" s="20">
+        <v>55.1</v>
+      </c>
+      <c r="Q27" s="20">
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="18">
+        <v>41</v>
+      </c>
+      <c r="B28" s="19">
+        <v>4104</v>
+      </c>
+      <c r="C28" s="19">
+        <v>3562</v>
+      </c>
+      <c r="D28" s="19">
+        <v>2366</v>
+      </c>
+      <c r="E28" s="20">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="F28" s="19">
+        <v>576</v>
+      </c>
+      <c r="G28" s="20">
+        <v>16.2</v>
+      </c>
+      <c r="H28" s="19">
+        <v>619</v>
+      </c>
+      <c r="I28" s="20">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J28" s="19">
+        <v>1878</v>
+      </c>
+      <c r="K28" s="20">
+        <v>52.7</v>
+      </c>
+      <c r="L28" s="19">
+        <v>1065</v>
+      </c>
+      <c r="M28" s="20">
+        <v>29.9</v>
+      </c>
+      <c r="N28" s="19">
+        <v>619</v>
+      </c>
+      <c r="O28" s="20">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="P28" s="20">
+        <v>57.7</v>
+      </c>
+      <c r="Q28" s="20">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="18">
+        <v>42</v>
+      </c>
+      <c r="B29" s="19">
+        <v>3851</v>
+      </c>
+      <c r="C29" s="19">
+        <v>3337</v>
+      </c>
+      <c r="D29" s="19">
+        <v>2306</v>
+      </c>
+      <c r="E29" s="20">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="F29" s="19">
+        <v>487</v>
+      </c>
+      <c r="G29" s="20">
+        <v>14.6</v>
+      </c>
+      <c r="H29" s="19">
+        <v>543</v>
+      </c>
+      <c r="I29" s="20">
+        <v>16.3</v>
+      </c>
+      <c r="J29" s="19">
+        <v>1841</v>
+      </c>
+      <c r="K29" s="20">
+        <v>55.2</v>
+      </c>
+      <c r="L29" s="19">
+        <v>949</v>
+      </c>
+      <c r="M29" s="20">
+        <v>28.4</v>
+      </c>
+      <c r="N29" s="19">
+        <v>547</v>
+      </c>
+      <c r="O29" s="20">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="P29" s="20">
+        <v>59.9</v>
+      </c>
+      <c r="Q29" s="20">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="18">
+        <v>43</v>
+      </c>
+      <c r="B30" s="19">
+        <v>3865</v>
+      </c>
+      <c r="C30" s="19">
+        <v>3336</v>
+      </c>
+      <c r="D30" s="19">
+        <v>2253</v>
+      </c>
+      <c r="E30" s="20">
+        <v>67.5</v>
+      </c>
+      <c r="F30" s="19">
+        <v>445</v>
+      </c>
+      <c r="G30" s="20">
+        <v>13.3</v>
+      </c>
+      <c r="H30" s="19">
+        <v>639</v>
+      </c>
+      <c r="I30" s="20">
+        <v>19.2</v>
+      </c>
+      <c r="J30" s="19">
+        <v>1803</v>
+      </c>
+      <c r="K30" s="20">
+        <v>54</v>
+      </c>
+      <c r="L30" s="19">
+        <v>898</v>
+      </c>
+      <c r="M30" s="20">
+        <v>26.9</v>
+      </c>
+      <c r="N30" s="19">
+        <v>635</v>
+      </c>
+      <c r="O30" s="20">
+        <v>19</v>
+      </c>
+      <c r="P30" s="20">
+        <v>58.3</v>
+      </c>
+      <c r="Q30" s="20">
+        <v>46.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="18">
+        <v>44</v>
+      </c>
+      <c r="B31" s="19">
+        <v>3760</v>
+      </c>
+      <c r="C31" s="19">
+        <v>3328</v>
+      </c>
+      <c r="D31" s="19">
+        <v>2223</v>
+      </c>
+      <c r="E31" s="20">
+        <v>66.8</v>
+      </c>
+      <c r="F31" s="19">
+        <v>424</v>
+      </c>
+      <c r="G31" s="20">
+        <v>12.7</v>
+      </c>
+      <c r="H31" s="19">
+        <v>682</v>
+      </c>
+      <c r="I31" s="20">
+        <v>20.5</v>
+      </c>
+      <c r="J31" s="19">
+        <v>1718</v>
+      </c>
+      <c r="K31" s="20">
+        <v>51.6</v>
+      </c>
+      <c r="L31" s="19">
+        <v>934</v>
+      </c>
+      <c r="M31" s="20">
+        <v>28</v>
+      </c>
+      <c r="N31" s="19">
+        <v>676</v>
+      </c>
+      <c r="O31" s="20">
+        <v>20.3</v>
+      </c>
+      <c r="P31" s="20">
+        <v>59.1</v>
+      </c>
+      <c r="Q31" s="20">
+        <v>45.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="18">
+        <v>45</v>
+      </c>
+      <c r="B32" s="19">
+        <v>3954</v>
+      </c>
+      <c r="C32" s="19">
+        <v>3456</v>
+      </c>
+      <c r="D32" s="19">
+        <v>2366</v>
+      </c>
+      <c r="E32" s="20">
+        <v>68.5</v>
+      </c>
+      <c r="F32" s="19">
+        <v>449</v>
+      </c>
+      <c r="G32" s="20">
+        <v>13</v>
+      </c>
+      <c r="H32" s="19">
+        <v>642</v>
+      </c>
+      <c r="I32" s="20">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J32" s="19">
+        <v>1820</v>
+      </c>
+      <c r="K32" s="20">
+        <v>52.7</v>
+      </c>
+      <c r="L32" s="19">
+        <v>990</v>
+      </c>
+      <c r="M32" s="20">
+        <v>28.6</v>
+      </c>
+      <c r="N32" s="19">
+        <v>646</v>
+      </c>
+      <c r="O32" s="20">
+        <v>18.7</v>
+      </c>
+      <c r="P32" s="20">
+        <v>59.8</v>
+      </c>
+      <c r="Q32" s="20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="18">
+        <v>46</v>
+      </c>
+      <c r="B33" s="19">
+        <v>3958</v>
+      </c>
+      <c r="C33" s="19">
+        <v>3514</v>
+      </c>
+      <c r="D33" s="19">
+        <v>2413</v>
+      </c>
+      <c r="E33" s="20">
+        <v>68.7</v>
+      </c>
+      <c r="F33" s="19">
+        <v>477</v>
+      </c>
+      <c r="G33" s="20">
+        <v>13.6</v>
+      </c>
+      <c r="H33" s="19">
+        <v>624</v>
+      </c>
+      <c r="I33" s="20">
+        <v>17.8</v>
+      </c>
+      <c r="J33" s="19">
+        <v>1955</v>
+      </c>
+      <c r="K33" s="20">
+        <v>55.6</v>
+      </c>
+      <c r="L33" s="19">
+        <v>973</v>
+      </c>
+      <c r="M33" s="20">
+        <v>27.7</v>
+      </c>
+      <c r="N33" s="19">
+        <v>585</v>
+      </c>
+      <c r="O33" s="20">
+        <v>16.7</v>
+      </c>
+      <c r="P33" s="20">
+        <v>61</v>
+      </c>
+      <c r="Q33" s="20">
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="18">
+        <v>47</v>
+      </c>
+      <c r="B34" s="19">
+        <v>3948</v>
+      </c>
+      <c r="C34" s="19">
+        <v>3548</v>
+      </c>
+      <c r="D34" s="19">
+        <v>2519</v>
+      </c>
+      <c r="E34" s="20">
+        <v>71</v>
+      </c>
+      <c r="F34" s="19">
+        <v>437</v>
+      </c>
+      <c r="G34" s="20">
+        <v>12.3</v>
+      </c>
+      <c r="H34" s="19">
+        <v>592</v>
+      </c>
+      <c r="I34" s="20">
+        <v>16.7</v>
+      </c>
+      <c r="J34" s="19">
+        <v>2058</v>
+      </c>
+      <c r="K34" s="20">
+        <v>58</v>
+      </c>
+      <c r="L34" s="19">
+        <v>936</v>
+      </c>
+      <c r="M34" s="20">
+        <v>26.4</v>
+      </c>
+      <c r="N34" s="19">
+        <v>554</v>
+      </c>
+      <c r="O34" s="20">
+        <v>15.6</v>
+      </c>
+      <c r="P34" s="20">
+        <v>63.8</v>
+      </c>
+      <c r="Q34" s="20">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="18">
+        <v>48</v>
+      </c>
+      <c r="B35" s="19">
+        <v>4285</v>
+      </c>
+      <c r="C35" s="19">
+        <v>3874</v>
+      </c>
+      <c r="D35" s="19">
+        <v>2733</v>
+      </c>
+      <c r="E35" s="20">
+        <v>70.5</v>
+      </c>
+      <c r="F35" s="19">
+        <v>489</v>
+      </c>
+      <c r="G35" s="20">
+        <v>12.6</v>
+      </c>
+      <c r="H35" s="19">
+        <v>652</v>
+      </c>
+      <c r="I35" s="20">
+        <v>16.8</v>
+      </c>
+      <c r="J35" s="19">
+        <v>2189</v>
+      </c>
+      <c r="K35" s="20">
+        <v>56.5</v>
+      </c>
+      <c r="L35" s="19">
+        <v>1034</v>
+      </c>
+      <c r="M35" s="20">
+        <v>26.7</v>
+      </c>
+      <c r="N35" s="19">
+        <v>651</v>
+      </c>
+      <c r="O35" s="20">
+        <v>16.8</v>
+      </c>
+      <c r="P35" s="20">
+        <v>63.8</v>
+      </c>
+      <c r="Q35" s="20">
+        <v>51.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="18">
+        <v>49</v>
+      </c>
+      <c r="B36" s="19">
+        <v>4284</v>
+      </c>
+      <c r="C36" s="19">
+        <v>3930</v>
+      </c>
+      <c r="D36" s="19">
+        <v>2740</v>
+      </c>
+      <c r="E36" s="20">
+        <v>69.7</v>
+      </c>
+      <c r="F36" s="19">
+        <v>476</v>
+      </c>
+      <c r="G36" s="20">
+        <v>12.1</v>
+      </c>
+      <c r="H36" s="19">
+        <v>714</v>
+      </c>
+      <c r="I36" s="20">
+        <v>18.2</v>
+      </c>
+      <c r="J36" s="19">
+        <v>2186</v>
+      </c>
+      <c r="K36" s="20">
+        <v>55.6</v>
+      </c>
+      <c r="L36" s="19">
+        <v>1031</v>
+      </c>
+      <c r="M36" s="20">
+        <v>26.2</v>
+      </c>
+      <c r="N36" s="19">
+        <v>712</v>
+      </c>
+      <c r="O36" s="20">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="P36" s="20">
+        <v>64</v>
+      </c>
+      <c r="Q36" s="20">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="18">
+        <v>50</v>
+      </c>
+      <c r="B37" s="19">
+        <v>4245</v>
+      </c>
+      <c r="C37" s="19">
+        <v>3849</v>
+      </c>
+      <c r="D37" s="19">
+        <v>2725</v>
+      </c>
+      <c r="E37" s="20">
+        <v>70.8</v>
+      </c>
+      <c r="F37" s="19">
+        <v>436</v>
+      </c>
+      <c r="G37" s="20">
+        <v>11.3</v>
+      </c>
+      <c r="H37" s="19">
+        <v>688</v>
+      </c>
+      <c r="I37" s="20">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="J37" s="19">
+        <v>2210</v>
+      </c>
+      <c r="K37" s="20">
+        <v>57.4</v>
+      </c>
+      <c r="L37" s="19">
+        <v>946</v>
+      </c>
+      <c r="M37" s="20">
+        <v>24.6</v>
+      </c>
+      <c r="N37" s="19">
+        <v>693</v>
+      </c>
+      <c r="O37" s="20">
+        <v>18</v>
+      </c>
+      <c r="P37" s="20">
+        <v>64.2</v>
+      </c>
+      <c r="Q37" s="20">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="18">
+        <v>51</v>
+      </c>
+      <c r="B38" s="19">
+        <v>4003</v>
+      </c>
+      <c r="C38" s="19">
+        <v>3588</v>
+      </c>
+      <c r="D38" s="19">
+        <v>2510</v>
+      </c>
+      <c r="E38" s="20">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="F38" s="19">
+        <v>468</v>
+      </c>
+      <c r="G38" s="20">
+        <v>13</v>
+      </c>
+      <c r="H38" s="19">
+        <v>610</v>
+      </c>
+      <c r="I38" s="20">
+        <v>17</v>
+      </c>
+      <c r="J38" s="19">
+        <v>2093</v>
+      </c>
+      <c r="K38" s="20">
+        <v>58.3</v>
+      </c>
+      <c r="L38" s="19">
+        <v>915</v>
+      </c>
+      <c r="M38" s="20">
+        <v>25.5</v>
+      </c>
+      <c r="N38" s="19">
+        <v>580</v>
+      </c>
+      <c r="O38" s="20">
+        <v>16.2</v>
+      </c>
+      <c r="P38" s="20">
+        <v>62.7</v>
+      </c>
+      <c r="Q38" s="20">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" s="18">
+        <v>52</v>
+      </c>
+      <c r="B39" s="19">
+        <v>4037</v>
+      </c>
+      <c r="C39" s="19">
+        <v>3759</v>
+      </c>
+      <c r="D39" s="19">
+        <v>2616</v>
+      </c>
+      <c r="E39" s="20">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="F39" s="19">
+        <v>480</v>
+      </c>
+      <c r="G39" s="20">
+        <v>12.8</v>
+      </c>
+      <c r="H39" s="19">
+        <v>663</v>
+      </c>
+      <c r="I39" s="20">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="J39" s="19">
+        <v>2175</v>
+      </c>
+      <c r="K39" s="20">
+        <v>57.9</v>
+      </c>
+      <c r="L39" s="19">
+        <v>959</v>
+      </c>
+      <c r="M39" s="20">
+        <v>25.5</v>
+      </c>
+      <c r="N39" s="19">
+        <v>624</v>
+      </c>
+      <c r="O39" s="20">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="P39" s="20">
+        <v>64.8</v>
+      </c>
+      <c r="Q39" s="20">
+        <v>53.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" s="18">
+        <v>53</v>
+      </c>
+      <c r="B40" s="19">
+        <v>3972</v>
+      </c>
+      <c r="C40" s="19">
+        <v>3644</v>
+      </c>
+      <c r="D40" s="19">
+        <v>2649</v>
+      </c>
+      <c r="E40" s="20">
+        <v>72.7</v>
+      </c>
+      <c r="F40" s="19">
+        <v>429</v>
+      </c>
+      <c r="G40" s="20">
+        <v>11.8</v>
+      </c>
+      <c r="H40" s="19">
+        <v>566</v>
+      </c>
+      <c r="I40" s="20">
+        <v>15.5</v>
+      </c>
+      <c r="J40" s="19">
+        <v>2180</v>
+      </c>
+      <c r="K40" s="20">
+        <v>59.8</v>
+      </c>
+      <c r="L40" s="19">
+        <v>910</v>
+      </c>
+      <c r="M40" s="20">
+        <v>25</v>
+      </c>
+      <c r="N40" s="19">
+        <v>554</v>
+      </c>
+      <c r="O40" s="20">
+        <v>15.2</v>
+      </c>
+      <c r="P40" s="20">
+        <v>66.7</v>
+      </c>
+      <c r="Q40" s="20">
+        <v>54.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" s="18">
+        <v>54</v>
+      </c>
+      <c r="B41" s="19">
+        <v>4333</v>
+      </c>
+      <c r="C41" s="19">
+        <v>4038</v>
+      </c>
+      <c r="D41" s="19">
+        <v>2871</v>
+      </c>
+      <c r="E41" s="20">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="F41" s="19">
+        <v>509</v>
+      </c>
+      <c r="G41" s="20">
+        <v>12.6</v>
+      </c>
+      <c r="H41" s="19">
+        <v>658</v>
+      </c>
+      <c r="I41" s="20">
+        <v>16.3</v>
+      </c>
+      <c r="J41" s="19">
+        <v>2322</v>
+      </c>
+      <c r="K41" s="20">
+        <v>57.5</v>
+      </c>
+      <c r="L41" s="19">
+        <v>1080</v>
+      </c>
+      <c r="M41" s="20">
+        <v>26.7</v>
+      </c>
+      <c r="N41" s="19">
+        <v>635</v>
+      </c>
+      <c r="O41" s="20">
+        <v>15.7</v>
+      </c>
+      <c r="P41" s="20">
+        <v>66.2</v>
+      </c>
+      <c r="Q41" s="20">
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" s="18">
+        <v>55</v>
+      </c>
+      <c r="B42" s="19">
+        <v>4435</v>
+      </c>
+      <c r="C42" s="19">
+        <v>4048</v>
+      </c>
+      <c r="D42" s="19">
+        <v>2848</v>
+      </c>
+      <c r="E42" s="20">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="F42" s="19">
+        <v>538</v>
+      </c>
+      <c r="G42" s="20">
+        <v>13.3</v>
+      </c>
+      <c r="H42" s="19">
+        <v>662</v>
+      </c>
+      <c r="I42" s="20">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J42" s="19">
+        <v>2321</v>
+      </c>
+      <c r="K42" s="20">
+        <v>57.3</v>
+      </c>
+      <c r="L42" s="19">
+        <v>1109</v>
+      </c>
+      <c r="M42" s="20">
+        <v>27.4</v>
+      </c>
+      <c r="N42" s="19">
+        <v>618</v>
+      </c>
+      <c r="O42" s="20">
+        <v>15.3</v>
+      </c>
+      <c r="P42" s="20">
+        <v>64.2</v>
+      </c>
+      <c r="Q42" s="20">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" s="18">
+        <v>56</v>
+      </c>
+      <c r="B43" s="19">
+        <v>4396</v>
+      </c>
+      <c r="C43" s="19">
+        <v>4135</v>
+      </c>
+      <c r="D43" s="19">
+        <v>2898</v>
+      </c>
+      <c r="E43" s="20">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F43" s="19">
+        <v>505</v>
+      </c>
+      <c r="G43" s="20">
+        <v>12.2</v>
+      </c>
+      <c r="H43" s="19">
+        <v>732</v>
+      </c>
+      <c r="I43" s="20">
+        <v>17.7</v>
+      </c>
+      <c r="J43" s="19">
+        <v>2403</v>
+      </c>
+      <c r="K43" s="20">
+        <v>58.1</v>
+      </c>
+      <c r="L43" s="19">
+        <v>1019</v>
+      </c>
+      <c r="M43" s="20">
+        <v>24.6</v>
+      </c>
+      <c r="N43" s="19">
+        <v>713</v>
+      </c>
+      <c r="O43" s="20">
+        <v>17.2</v>
+      </c>
+      <c r="P43" s="20">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="Q43" s="20">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
+        <v>57</v>
+      </c>
+      <c r="B44" s="19">
+        <v>4428</v>
+      </c>
+      <c r="C44" s="19">
+        <v>4197</v>
+      </c>
+      <c r="D44" s="19">
+        <v>2990</v>
+      </c>
+      <c r="E44" s="20">
+        <v>71.2</v>
+      </c>
+      <c r="F44" s="19">
+        <v>500</v>
+      </c>
+      <c r="G44" s="20">
+        <v>11.9</v>
+      </c>
+      <c r="H44" s="19">
+        <v>707</v>
+      </c>
+      <c r="I44" s="20">
+        <v>16.8</v>
+      </c>
+      <c r="J44" s="19">
+        <v>2499</v>
+      </c>
+      <c r="K44" s="20">
+        <v>59.5</v>
+      </c>
+      <c r="L44" s="19">
+        <v>1011</v>
+      </c>
+      <c r="M44" s="20">
+        <v>24.1</v>
+      </c>
+      <c r="N44" s="19">
+        <v>687</v>
+      </c>
+      <c r="O44" s="20">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="P44" s="20">
+        <v>67.5</v>
+      </c>
+      <c r="Q44" s="20">
+        <v>56.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" s="18">
+        <v>58</v>
+      </c>
+      <c r="B45" s="19">
+        <v>4564</v>
+      </c>
+      <c r="C45" s="19">
+        <v>4323</v>
+      </c>
+      <c r="D45" s="19">
+        <v>3086</v>
+      </c>
+      <c r="E45" s="20">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="F45" s="19">
+        <v>502</v>
+      </c>
+      <c r="G45" s="20">
+        <v>11.6</v>
+      </c>
+      <c r="H45" s="19">
+        <v>735</v>
+      </c>
+      <c r="I45" s="20">
+        <v>17</v>
+      </c>
+      <c r="J45" s="19">
+        <v>2627</v>
+      </c>
+      <c r="K45" s="20">
+        <v>60.8</v>
+      </c>
+      <c r="L45" s="19">
+        <v>964</v>
+      </c>
+      <c r="M45" s="20">
+        <v>22.3</v>
+      </c>
+      <c r="N45" s="19">
+        <v>732</v>
+      </c>
+      <c r="O45" s="20">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="P45" s="20">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="Q45" s="20">
+        <v>57.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" s="18">
+        <v>59</v>
+      </c>
+      <c r="B46" s="19">
+        <v>4029</v>
+      </c>
+      <c r="C46" s="19">
+        <v>3800</v>
+      </c>
+      <c r="D46" s="19">
+        <v>2714</v>
+      </c>
+      <c r="E46" s="20">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="F46" s="19">
+        <v>451</v>
+      </c>
+      <c r="G46" s="20">
+        <v>11.9</v>
+      </c>
+      <c r="H46" s="19">
+        <v>634</v>
+      </c>
+      <c r="I46" s="20">
+        <v>16.7</v>
+      </c>
+      <c r="J46" s="19">
+        <v>2302</v>
+      </c>
+      <c r="K46" s="20">
+        <v>60.6</v>
+      </c>
+      <c r="L46" s="19">
+        <v>883</v>
+      </c>
+      <c r="M46" s="20">
+        <v>23.2</v>
+      </c>
+      <c r="N46" s="19">
+        <v>615</v>
+      </c>
+      <c r="O46" s="20">
+        <v>16.2</v>
+      </c>
+      <c r="P46" s="20">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="Q46" s="20">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" s="18">
+        <v>60</v>
+      </c>
+      <c r="B47" s="19">
+        <v>4183</v>
+      </c>
+      <c r="C47" s="19">
+        <v>3939</v>
+      </c>
+      <c r="D47" s="19">
+        <v>2888</v>
+      </c>
+      <c r="E47" s="20">
+        <v>73.3</v>
+      </c>
+      <c r="F47" s="19">
+        <v>428</v>
+      </c>
+      <c r="G47" s="20">
+        <v>10.9</v>
+      </c>
+      <c r="H47" s="19">
+        <v>623</v>
+      </c>
+      <c r="I47" s="20">
+        <v>15.8</v>
+      </c>
+      <c r="J47" s="19">
+        <v>2509</v>
+      </c>
+      <c r="K47" s="20">
+        <v>63.7</v>
+      </c>
+      <c r="L47" s="19">
+        <v>810</v>
+      </c>
+      <c r="M47" s="20">
+        <v>20.6</v>
+      </c>
+      <c r="N47" s="19">
+        <v>620</v>
+      </c>
+      <c r="O47" s="20">
+        <v>15.7</v>
+      </c>
+      <c r="P47" s="20">
+        <v>69</v>
+      </c>
+      <c r="Q47" s="20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="18">
+        <v>61</v>
+      </c>
+      <c r="B48" s="19">
+        <v>4415</v>
+      </c>
+      <c r="C48" s="19">
+        <v>4175</v>
+      </c>
+      <c r="D48" s="19">
+        <v>3035</v>
+      </c>
+      <c r="E48" s="20">
+        <v>72.7</v>
+      </c>
+      <c r="F48" s="19">
+        <v>457</v>
+      </c>
+      <c r="G48" s="20">
+        <v>11</v>
+      </c>
+      <c r="H48" s="19">
+        <v>683</v>
+      </c>
+      <c r="I48" s="20">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J48" s="19">
+        <v>2580</v>
+      </c>
+      <c r="K48" s="20">
+        <v>61.8</v>
+      </c>
+      <c r="L48" s="19">
+        <v>932</v>
+      </c>
+      <c r="M48" s="20">
+        <v>22.3</v>
+      </c>
+      <c r="N48" s="19">
+        <v>663</v>
+      </c>
+      <c r="O48" s="20">
+        <v>15.9</v>
+      </c>
+      <c r="P48" s="20">
+        <v>68.7</v>
+      </c>
+      <c r="Q48" s="20">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49" s="18">
+        <v>62</v>
+      </c>
+      <c r="B49" s="19">
+        <v>3938</v>
+      </c>
+      <c r="C49" s="19">
+        <v>3724</v>
+      </c>
+      <c r="D49" s="19">
+        <v>2764</v>
+      </c>
+      <c r="E49" s="20">
+        <v>74.2</v>
+      </c>
+      <c r="F49" s="19">
+        <v>409</v>
+      </c>
+      <c r="G49" s="20">
+        <v>11</v>
+      </c>
+      <c r="H49" s="19">
+        <v>551</v>
+      </c>
+      <c r="I49" s="20">
+        <v>14.8</v>
+      </c>
+      <c r="J49" s="19">
+        <v>2409</v>
+      </c>
+      <c r="K49" s="20">
+        <v>64.7</v>
+      </c>
+      <c r="L49" s="19">
+        <v>771</v>
+      </c>
+      <c r="M49" s="20">
+        <v>20.7</v>
+      </c>
+      <c r="N49" s="19">
+        <v>545</v>
+      </c>
+      <c r="O49" s="20">
+        <v>14.6</v>
+      </c>
+      <c r="P49" s="20">
+        <v>70.2</v>
+      </c>
+      <c r="Q49" s="20">
+        <v>61.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" s="18">
+        <v>63</v>
+      </c>
+      <c r="B50" s="19">
+        <v>3885</v>
+      </c>
+      <c r="C50" s="19">
+        <v>3714</v>
+      </c>
+      <c r="D50" s="19">
+        <v>2775</v>
+      </c>
+      <c r="E50" s="20">
+        <v>74.7</v>
+      </c>
+      <c r="F50" s="19">
+        <v>350</v>
+      </c>
+      <c r="G50" s="20">
+        <v>9.4</v>
+      </c>
+      <c r="H50" s="19">
+        <v>590</v>
+      </c>
+      <c r="I50" s="20">
+        <v>15.9</v>
+      </c>
+      <c r="J50" s="19">
+        <v>2446</v>
+      </c>
+      <c r="K50" s="20">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="L50" s="19">
+        <v>702</v>
+      </c>
+      <c r="M50" s="20">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="N50" s="19">
+        <v>565</v>
+      </c>
+      <c r="O50" s="20">
+        <v>15.2</v>
+      </c>
+      <c r="P50" s="20">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="Q50" s="20">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51" s="18">
+        <v>64</v>
+      </c>
+      <c r="B51" s="19">
+        <v>3984</v>
+      </c>
+      <c r="C51" s="19">
+        <v>3831</v>
+      </c>
+      <c r="D51" s="19">
+        <v>2894</v>
+      </c>
+      <c r="E51" s="20">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="F51" s="19">
+        <v>360</v>
+      </c>
+      <c r="G51" s="20">
+        <v>9.4</v>
+      </c>
+      <c r="H51" s="19">
+        <v>576</v>
+      </c>
+      <c r="I51" s="20">
+        <v>15</v>
+      </c>
+      <c r="J51" s="19">
+        <v>2545</v>
+      </c>
+      <c r="K51" s="20">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="L51" s="19">
+        <v>729</v>
+      </c>
+      <c r="M51" s="20">
+        <v>19</v>
+      </c>
+      <c r="N51" s="19">
+        <v>556</v>
+      </c>
+      <c r="O51" s="20">
+        <v>14.5</v>
+      </c>
+      <c r="P51" s="20">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="Q51" s="20">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52" s="18">
+        <v>65</v>
+      </c>
+      <c r="B52" s="19">
+        <v>3552</v>
+      </c>
+      <c r="C52" s="19">
+        <v>3401</v>
+      </c>
+      <c r="D52" s="19">
+        <v>2571</v>
+      </c>
+      <c r="E52" s="20">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="F52" s="19">
+        <v>315</v>
+      </c>
+      <c r="G52" s="20">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H52" s="19">
+        <v>515</v>
+      </c>
+      <c r="I52" s="20">
+        <v>15.1</v>
+      </c>
+      <c r="J52" s="19">
+        <v>2319</v>
+      </c>
+      <c r="K52" s="20">
+        <v>68.2</v>
+      </c>
+      <c r="L52" s="19">
+        <v>588</v>
+      </c>
+      <c r="M52" s="20">
+        <v>17.3</v>
+      </c>
+      <c r="N52" s="19">
+        <v>495</v>
+      </c>
+      <c r="O52" s="20">
+        <v>14.5</v>
+      </c>
+      <c r="P52" s="20">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="Q52" s="20">
+        <v>65.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53" s="18">
+        <v>66</v>
+      </c>
+      <c r="B53" s="19">
+        <v>3576</v>
+      </c>
+      <c r="C53" s="19">
+        <v>3459</v>
+      </c>
+      <c r="D53" s="19">
+        <v>2696</v>
+      </c>
+      <c r="E53" s="20">
+        <v>78</v>
+      </c>
+      <c r="F53" s="19">
+        <v>280</v>
+      </c>
+      <c r="G53" s="20">
+        <v>8.1</v>
+      </c>
+      <c r="H53" s="19">
+        <v>483</v>
+      </c>
+      <c r="I53" s="20">
+        <v>14</v>
+      </c>
+      <c r="J53" s="19">
+        <v>2366</v>
+      </c>
+      <c r="K53" s="20">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="L53" s="19">
+        <v>620</v>
+      </c>
+      <c r="M53" s="20">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="N53" s="19">
+        <v>473</v>
+      </c>
+      <c r="O53" s="20">
+        <v>13.7</v>
+      </c>
+      <c r="P53" s="20">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="Q53" s="20">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54" s="18">
+        <v>67</v>
+      </c>
+      <c r="B54" s="19">
+        <v>3517</v>
+      </c>
+      <c r="C54" s="19">
+        <v>3389</v>
+      </c>
+      <c r="D54" s="19">
+        <v>2673</v>
+      </c>
+      <c r="E54" s="20">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="F54" s="19">
+        <v>277</v>
+      </c>
+      <c r="G54" s="20">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H54" s="19">
+        <v>439</v>
+      </c>
+      <c r="I54" s="20">
+        <v>12.9</v>
+      </c>
+      <c r="J54" s="19">
+        <v>2376</v>
+      </c>
+      <c r="K54" s="20">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="L54" s="19">
+        <v>592</v>
+      </c>
+      <c r="M54" s="20">
+        <v>17.5</v>
+      </c>
+      <c r="N54" s="19">
+        <v>422</v>
+      </c>
+      <c r="O54" s="20">
+        <v>12.4</v>
+      </c>
+      <c r="P54" s="20">
+        <v>76</v>
+      </c>
+      <c r="Q54" s="20">
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55" s="18">
+        <v>68</v>
+      </c>
+      <c r="B55" s="19">
+        <v>3083</v>
+      </c>
+      <c r="C55" s="19">
+        <v>3005</v>
+      </c>
+      <c r="D55" s="19">
+        <v>2265</v>
+      </c>
+      <c r="E55" s="20">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="F55" s="19">
+        <v>325</v>
+      </c>
+      <c r="G55" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="H55" s="19">
+        <v>415</v>
+      </c>
+      <c r="I55" s="20">
+        <v>13.8</v>
+      </c>
+      <c r="J55" s="19">
+        <v>2037</v>
+      </c>
+      <c r="K55" s="20">
+        <v>67.8</v>
+      </c>
+      <c r="L55" s="19">
+        <v>564</v>
+      </c>
+      <c r="M55" s="20">
+        <v>18.8</v>
+      </c>
+      <c r="N55" s="19">
+        <v>404</v>
+      </c>
+      <c r="O55" s="20">
+        <v>13.5</v>
+      </c>
+      <c r="P55" s="20">
+        <v>73.5</v>
+      </c>
+      <c r="Q55" s="20">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56" s="18">
+        <v>69</v>
+      </c>
+      <c r="B56" s="19">
+        <v>3301</v>
+      </c>
+      <c r="C56" s="19">
+        <v>3155</v>
+      </c>
+      <c r="D56" s="19">
+        <v>2466</v>
+      </c>
+      <c r="E56" s="20">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="F56" s="19">
+        <v>265</v>
+      </c>
+      <c r="G56" s="20">
+        <v>8.4</v>
+      </c>
+      <c r="H56" s="19">
+        <v>425</v>
+      </c>
+      <c r="I56" s="20">
+        <v>13.5</v>
+      </c>
+      <c r="J56" s="19">
+        <v>2197</v>
+      </c>
+      <c r="K56" s="20">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="L56" s="19">
+        <v>549</v>
+      </c>
+      <c r="M56" s="20">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="N56" s="19">
+        <v>410</v>
+      </c>
+      <c r="O56" s="20">
+        <v>13</v>
+      </c>
+      <c r="P56" s="20">
+        <v>74.7</v>
+      </c>
+      <c r="Q56" s="20">
+        <v>66.599999999999994</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57" s="18">
+        <v>70</v>
+      </c>
+      <c r="B57" s="19">
+        <v>3146</v>
+      </c>
+      <c r="C57" s="19">
+        <v>3019</v>
+      </c>
+      <c r="D57" s="19">
+        <v>2244</v>
+      </c>
+      <c r="E57" s="20">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="F57" s="19">
+        <v>279</v>
+      </c>
+      <c r="G57" s="20">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H57" s="19">
+        <v>495</v>
+      </c>
+      <c r="I57" s="20">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J57" s="19">
+        <v>1991</v>
+      </c>
+      <c r="K57" s="20">
+        <v>66</v>
+      </c>
+      <c r="L57" s="19">
+        <v>560</v>
+      </c>
+      <c r="M57" s="20">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="N57" s="19">
+        <v>467</v>
+      </c>
+      <c r="O57" s="20">
+        <v>15.5</v>
+      </c>
+      <c r="P57" s="20">
+        <v>71.3</v>
+      </c>
+      <c r="Q57" s="20">
+        <v>63.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A58" s="18">
+        <v>71</v>
+      </c>
+      <c r="B58" s="19">
+        <v>3240</v>
+      </c>
+      <c r="C58" s="19">
+        <v>3115</v>
+      </c>
+      <c r="D58" s="19">
+        <v>2430</v>
+      </c>
+      <c r="E58" s="20">
+        <v>78</v>
+      </c>
+      <c r="F58" s="19">
+        <v>301</v>
+      </c>
+      <c r="G58" s="20">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H58" s="19">
+        <v>383</v>
+      </c>
+      <c r="I58" s="20">
+        <v>12.3</v>
+      </c>
+      <c r="J58" s="19">
+        <v>2118</v>
+      </c>
+      <c r="K58" s="20">
+        <v>68</v>
+      </c>
+      <c r="L58" s="19">
+        <v>635</v>
+      </c>
+      <c r="M58" s="20">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="N58" s="19">
+        <v>362</v>
+      </c>
+      <c r="O58" s="20">
+        <v>11.6</v>
+      </c>
+      <c r="P58" s="20">
+        <v>75</v>
+      </c>
+      <c r="Q58" s="20">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A59" s="18">
+        <v>72</v>
+      </c>
+      <c r="B59" s="19">
+        <v>2778</v>
+      </c>
+      <c r="C59" s="19">
+        <v>2667</v>
+      </c>
+      <c r="D59" s="19">
+        <v>2008</v>
+      </c>
+      <c r="E59" s="20">
+        <v>75.3</v>
+      </c>
+      <c r="F59" s="19">
+        <v>249</v>
+      </c>
+      <c r="G59" s="20">
+        <v>9.4</v>
+      </c>
+      <c r="H59" s="19">
+        <v>410</v>
+      </c>
+      <c r="I59" s="20">
+        <v>15.4</v>
+      </c>
+      <c r="J59" s="19">
+        <v>1780</v>
+      </c>
+      <c r="K59" s="20">
+        <v>66.7</v>
+      </c>
+      <c r="L59" s="19">
+        <v>478</v>
+      </c>
+      <c r="M59" s="20">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="N59" s="19">
+        <v>409</v>
+      </c>
+      <c r="O59" s="20">
+        <v>15.3</v>
+      </c>
+      <c r="P59" s="20">
+        <v>72.3</v>
+      </c>
+      <c r="Q59" s="20">
+        <v>64.099999999999994</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A60" s="18">
+        <v>73</v>
+      </c>
+      <c r="B60" s="19">
+        <v>2329</v>
+      </c>
+      <c r="C60" s="19">
+        <v>2228</v>
+      </c>
+      <c r="D60" s="19">
+        <v>1716</v>
+      </c>
+      <c r="E60" s="20">
+        <v>77</v>
+      </c>
+      <c r="F60" s="19">
+        <v>186</v>
+      </c>
+      <c r="G60" s="20">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H60" s="19">
+        <v>327</v>
+      </c>
+      <c r="I60" s="20">
+        <v>14.7</v>
+      </c>
+      <c r="J60" s="19">
+        <v>1541</v>
+      </c>
+      <c r="K60" s="20">
+        <v>69.2</v>
+      </c>
+      <c r="L60" s="19">
+        <v>381</v>
+      </c>
+      <c r="M60" s="20">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="N60" s="19">
+        <v>306</v>
+      </c>
+      <c r="O60" s="20">
+        <v>13.7</v>
+      </c>
+      <c r="P60" s="20">
+        <v>73.7</v>
+      </c>
+      <c r="Q60" s="20">
+        <v>66.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A61" s="18">
+        <v>74</v>
+      </c>
+      <c r="B61" s="19">
+        <v>2176</v>
+      </c>
+      <c r="C61" s="19">
+        <v>2096</v>
+      </c>
+      <c r="D61" s="19">
+        <v>1619</v>
+      </c>
+      <c r="E61" s="20">
+        <v>77.3</v>
+      </c>
+      <c r="F61" s="19">
+        <v>164</v>
+      </c>
+      <c r="G61" s="20">
+        <v>7.8</v>
+      </c>
+      <c r="H61" s="19">
+        <v>312</v>
+      </c>
+      <c r="I61" s="20">
+        <v>14.9</v>
+      </c>
+      <c r="J61" s="19">
+        <v>1403</v>
+      </c>
+      <c r="K61" s="20">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="L61" s="19">
+        <v>376</v>
+      </c>
+      <c r="M61" s="20">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="N61" s="19">
+        <v>318</v>
+      </c>
+      <c r="O61" s="20">
+        <v>15.2</v>
+      </c>
+      <c r="P61" s="20">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="Q61" s="20">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A62" s="18">
+        <v>75</v>
+      </c>
+      <c r="B62" s="19">
+        <v>2346</v>
+      </c>
+      <c r="C62" s="19">
+        <v>2280</v>
+      </c>
+      <c r="D62" s="19">
+        <v>1792</v>
+      </c>
+      <c r="E62" s="20">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="F62" s="19">
+        <v>157</v>
+      </c>
+      <c r="G62" s="20">
+        <v>6.9</v>
+      </c>
+      <c r="H62" s="19">
+        <v>331</v>
+      </c>
+      <c r="I62" s="20">
+        <v>14.5</v>
+      </c>
+      <c r="J62" s="19">
+        <v>1607</v>
+      </c>
+      <c r="K62" s="20">
+        <v>70.5</v>
+      </c>
+      <c r="L62" s="19">
+        <v>345</v>
+      </c>
+      <c r="M62" s="20">
+        <v>15.2</v>
+      </c>
+      <c r="N62" s="19">
+        <v>327</v>
+      </c>
+      <c r="O62" s="20">
+        <v>14.4</v>
+      </c>
+      <c r="P62" s="20">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="Q62" s="20">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A63" s="18">
+        <v>76</v>
+      </c>
+      <c r="B63" s="19">
+        <v>1904</v>
+      </c>
+      <c r="C63" s="19">
+        <v>1855</v>
+      </c>
+      <c r="D63" s="19">
+        <v>1493</v>
+      </c>
+      <c r="E63" s="20">
+        <v>80.5</v>
+      </c>
+      <c r="F63" s="19">
+        <v>134</v>
+      </c>
+      <c r="G63" s="20">
+        <v>7.2</v>
+      </c>
+      <c r="H63" s="19">
+        <v>227</v>
+      </c>
+      <c r="I63" s="20">
+        <v>12.3</v>
+      </c>
+      <c r="J63" s="19">
+        <v>1322</v>
+      </c>
+      <c r="K63" s="20">
+        <v>71.3</v>
+      </c>
+      <c r="L63" s="19">
+        <v>301</v>
+      </c>
+      <c r="M63" s="20">
+        <v>16.2</v>
+      </c>
+      <c r="N63" s="19">
+        <v>232</v>
+      </c>
+      <c r="O63" s="20">
+        <v>12.5</v>
+      </c>
+      <c r="P63" s="20">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="Q63" s="20">
+        <v>69.400000000000006</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A64" s="18">
+        <v>77</v>
+      </c>
+      <c r="B64" s="19">
+        <v>1863</v>
+      </c>
+      <c r="C64" s="19">
+        <v>1804</v>
+      </c>
+      <c r="D64" s="19">
+        <v>1452</v>
+      </c>
+      <c r="E64" s="20">
+        <v>80.5</v>
+      </c>
+      <c r="F64" s="19">
+        <v>128</v>
+      </c>
+      <c r="G64" s="20">
+        <v>7.1</v>
+      </c>
+      <c r="H64" s="19">
+        <v>224</v>
+      </c>
+      <c r="I64" s="20">
+        <v>12.4</v>
+      </c>
+      <c r="J64" s="19">
+        <v>1270</v>
+      </c>
+      <c r="K64" s="20">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="L64" s="19">
+        <v>313</v>
+      </c>
+      <c r="M64" s="20">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="N64" s="19">
+        <v>220</v>
+      </c>
+      <c r="O64" s="20">
+        <v>12.2</v>
+      </c>
+      <c r="P64" s="20">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="Q64" s="20">
+        <v>68.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" s="18">
+        <v>78</v>
+      </c>
+      <c r="B65" s="19">
+        <v>1719</v>
+      </c>
+      <c r="C65" s="19">
+        <v>1688</v>
+      </c>
+      <c r="D65" s="19">
+        <v>1259</v>
+      </c>
+      <c r="E65" s="20">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="F65" s="19">
+        <v>182</v>
+      </c>
+      <c r="G65" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="H65" s="19">
+        <v>248</v>
+      </c>
+      <c r="I65" s="20">
+        <v>14.7</v>
+      </c>
+      <c r="J65" s="19">
+        <v>1074</v>
+      </c>
+      <c r="K65" s="20">
+        <v>63.6</v>
+      </c>
+      <c r="L65" s="19">
+        <v>387</v>
+      </c>
+      <c r="M65" s="20">
+        <v>22.9</v>
+      </c>
+      <c r="N65" s="19">
+        <v>228</v>
+      </c>
+      <c r="O65" s="20">
+        <v>13.5</v>
+      </c>
+      <c r="P65" s="20">
+        <v>73.2</v>
+      </c>
+      <c r="Q65" s="20">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66" s="18">
+        <v>79</v>
+      </c>
+      <c r="B66" s="19">
+        <v>1501</v>
+      </c>
+      <c r="C66" s="19">
+        <v>1422</v>
+      </c>
+      <c r="D66" s="19">
+        <v>1104</v>
+      </c>
+      <c r="E66" s="20">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="F66" s="19">
+        <v>132</v>
+      </c>
+      <c r="G66" s="20">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H66" s="19">
+        <v>186</v>
+      </c>
+      <c r="I66" s="20">
+        <v>13.1</v>
+      </c>
+      <c r="J66" s="19">
+        <v>952</v>
+      </c>
+      <c r="K66" s="20">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="L66" s="19">
+        <v>297</v>
+      </c>
+      <c r="M66" s="20">
+        <v>20.9</v>
+      </c>
+      <c r="N66" s="19">
+        <v>173</v>
+      </c>
+      <c r="O66" s="20">
+        <v>12.1</v>
+      </c>
+      <c r="P66" s="20">
+        <v>73.5</v>
+      </c>
+      <c r="Q66" s="20">
+        <v>63.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A67" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B67" s="19">
+        <v>6098</v>
+      </c>
+      <c r="C67" s="19">
+        <v>5879</v>
+      </c>
+      <c r="D67" s="19">
+        <v>4418</v>
+      </c>
+      <c r="E67" s="20">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="F67" s="19">
+        <v>535</v>
+      </c>
+      <c r="G67" s="20">
+        <v>9.1</v>
+      </c>
+      <c r="H67" s="19">
+        <v>926</v>
+      </c>
+      <c r="I67" s="20">
+        <v>15.8</v>
+      </c>
+      <c r="J67" s="19">
+        <v>3764</v>
+      </c>
+      <c r="K67" s="20">
+        <v>64</v>
+      </c>
+      <c r="L67" s="19">
+        <v>1223</v>
+      </c>
+      <c r="M67" s="20">
+        <v>20.8</v>
+      </c>
+      <c r="N67" s="19">
+        <v>892</v>
+      </c>
+      <c r="O67" s="20">
+        <v>15.2</v>
+      </c>
+      <c r="P67" s="20">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="Q67" s="20">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B68" s="19">
+        <v>5796</v>
+      </c>
+      <c r="C68" s="19">
+        <v>5651</v>
+      </c>
+      <c r="D68" s="19">
+        <v>3862</v>
+      </c>
+      <c r="E68" s="20">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="F68" s="19">
+        <v>598</v>
+      </c>
+      <c r="G68" s="20">
+        <v>10.6</v>
+      </c>
+      <c r="H68" s="19">
+        <v>1191</v>
+      </c>
+      <c r="I68" s="20">
+        <v>21.1</v>
+      </c>
+      <c r="J68" s="19">
+        <v>3023</v>
+      </c>
+      <c r="K68" s="20">
+        <v>53.5</v>
+      </c>
+      <c r="L68" s="19">
+        <v>1529</v>
+      </c>
+      <c r="M68" s="20">
+        <v>27.1</v>
+      </c>
+      <c r="N68" s="19">
+        <v>1099</v>
+      </c>
+      <c r="O68" s="20">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="P68" s="20">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="Q68" s="20">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A69" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B69" s="22">
+        <v>11894</v>
+      </c>
+      <c r="C69" s="22">
+        <v>11530</v>
+      </c>
+      <c r="D69" s="22">
+        <v>8280</v>
+      </c>
+      <c r="E69" s="22">
+        <v>71.812662619254127</v>
+      </c>
+      <c r="F69" s="22">
+        <v>1133</v>
+      </c>
+      <c r="G69" s="22">
+        <v>9.8265394622723345</v>
+      </c>
+      <c r="H69" s="22">
+        <v>2117</v>
+      </c>
+      <c r="I69" s="22">
+        <v>18.360797918473548</v>
+      </c>
+      <c r="J69" s="22">
+        <v>6787</v>
+      </c>
+      <c r="K69" s="22">
+        <v>58.863833477883787</v>
+      </c>
+      <c r="L69" s="22">
+        <v>2752</v>
+      </c>
+      <c r="M69" s="22">
+        <v>23.868169991326972</v>
+      </c>
+      <c r="N69" s="22">
+        <v>1991</v>
+      </c>
+      <c r="O69" s="22">
+        <v>17.267996530789244</v>
+      </c>
+      <c r="P69" s="22">
+        <v>69.614931898436183</v>
+      </c>
+      <c r="Q69" s="22">
+        <v>57.062384395493524</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8586DA17-D321-4EF1-971D-C0B93F6A8DBC}">
   <dimension ref="B26:G31"/>
   <sheetViews>
@@ -4489,7 +8362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE3A6B8-3B6F-4BB0-983B-71CAF56E2298}">
   <dimension ref="A1:J102"/>
   <sheetViews>
@@ -7768,7 +11641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E255563-698D-424C-803C-B80D00E8EAF1}">
   <dimension ref="A1:F6"/>
   <sheetViews>

</xml_diff>